<commit_message>
fix(infrastructure-be): final rule seed data
</commit_message>
<xml_diff>
--- a/apps/server/infrastructure-be/src/modules/seeders/seedData.xlsx
+++ b/apps/server/infrastructure-be/src/modules/seeders/seedData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="117">
   <si>
     <t>operator</t>
   </si>
@@ -231,27 +231,9 @@
     <t>Rule sixteen</t>
   </si>
   <si>
-    <t>Rule 18</t>
-  </si>
-  <si>
-    <t>Rule 19</t>
-  </si>
-  <si>
-    <t>Rule 20</t>
-  </si>
-  <si>
-    <t>Rule 21</t>
-  </si>
-  <si>
     <t>Marginalized Group</t>
   </si>
   <si>
-    <t>Rule 22</t>
-  </si>
-  <si>
-    <t>Rule 23</t>
-  </si>
-  <si>
     <t>Rule seventeen</t>
   </si>
   <si>
@@ -295,6 +277,96 @@
   </si>
   <si>
     <t>valueThreshold</t>
+  </si>
+  <si>
+    <t>Change in supplier availability due to unforeseen events (e.g., natural disasters, economic crises).</t>
+  </si>
+  <si>
+    <t>Changes in project financing necessitating a reevaluation of procurement strategies.</t>
+  </si>
+  <si>
+    <t>Legal challenges or concerns regarding the open tendering process.</t>
+  </si>
+  <si>
+    <t>Change in market conditions, leading to a lack of competition.</t>
+  </si>
+  <si>
+    <t>Emergence of new, more qualified suppliers after the initial tender announcement.</t>
+  </si>
+  <si>
+    <t>Unexpected changes in project scope or specifications.</t>
+  </si>
+  <si>
+    <t>Introduction of new technology or methodologies that require expertise from a broader range of suppliers.</t>
+  </si>
+  <si>
+    <t>Changes in government policies or regulations affecting supplier selection criteria.</t>
+  </si>
+  <si>
+    <t>Internal organizational changes impacting the composition of the supplier pool.</t>
+  </si>
+  <si>
+    <t>Identification of additional qualified suppliers after the initial selection.</t>
+  </si>
+  <si>
+    <t>Changes in project requirements necessitating a broader pool of suppliers.</t>
+  </si>
+  <si>
+    <t>Legal challenges or concerns regarding the selectivity criteria.</t>
+  </si>
+  <si>
+    <t>Emergence of innovative solutions or technologies that prompt a reassessment of proposal requirements.</t>
+  </si>
+  <si>
+    <t>Changes in project stakeholders or decision-makers necessitating a reevaluation of criteria.</t>
+  </si>
+  <si>
+    <t>Internal capacity-building initiatives requiring a more detailed proposal review.</t>
+  </si>
+  <si>
+    <t>Need for a more detailed proposal evaluation due to project complexity.</t>
+  </si>
+  <si>
+    <t>Changes in project scope or requirements that necessitate a new proposal.</t>
+  </si>
+  <si>
+    <t>Legal challenges or concerns regarding the RFP process.</t>
+  </si>
+  <si>
+    <t>Changes in supplier capacity or reliability affecting the single-source decision.</t>
+  </si>
+  <si>
+    <t>Shift in the organization's risk tolerance or risk management approach.</t>
+  </si>
+  <si>
+    <t>External pressures or legal challenges prompting a reevaluation of the direct procurement method.</t>
+  </si>
+  <si>
+    <t>Identification of additional qualified suppliers after the initial decision.</t>
+  </si>
+  <si>
+    <t>Changes in project scope or specifications requiring a new procurement approach.</t>
+  </si>
+  <si>
+    <t>Legal challenges or concerns regarding the direct procurement decision.</t>
+  </si>
+  <si>
+    <t>Rule eighteen</t>
+  </si>
+  <si>
+    <t>Rule nineteen</t>
+  </si>
+  <si>
+    <t>Rule twenty</t>
+  </si>
+  <si>
+    <t>Rule twentyone</t>
+  </si>
+  <si>
+    <t>Rule twentytwo</t>
+  </si>
+  <si>
+    <t>Rule Twentythree</t>
   </si>
 </sst>
 </file>
@@ -338,12 +410,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,16 +720,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S94"/>
+  <dimension ref="A1:S103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
     <col min="3" max="3" width="7.21875" customWidth="1"/>
     <col min="4" max="4" width="26.88671875" customWidth="1"/>
     <col min="5" max="5" width="6.21875" customWidth="1"/>
@@ -710,19 +785,19 @@
         <v>52</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -763,13 +838,13 @@
         <v>5</v>
       </c>
       <c r="P2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="Q2" t="b">
         <v>1</v>
       </c>
       <c r="S2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -780,7 +855,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -798,13 +873,13 @@
         <v>5</v>
       </c>
       <c r="K3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="L3" t="s">
         <v>1</v>
       </c>
       <c r="S3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -815,7 +890,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -830,7 +905,7 @@
         <v>4</v>
       </c>
       <c r="S4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
@@ -866,7 +941,7 @@
         <v>2</v>
       </c>
       <c r="S6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
@@ -877,7 +952,7 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -892,7 +967,7 @@
         <v>4</v>
       </c>
       <c r="S7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
@@ -903,7 +978,7 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -918,7 +993,7 @@
         <v>4</v>
       </c>
       <c r="S8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
@@ -962,7 +1037,7 @@
         <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -985,7 +1060,7 @@
         <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
@@ -1042,10 +1117,13 @@
         <v>5</v>
       </c>
       <c r="P14" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="Q14" t="b">
         <v>1</v>
+      </c>
+      <c r="S14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1056,7 +1134,7 @@
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
@@ -1069,6 +1147,9 @@
       </c>
       <c r="H15" t="s">
         <v>4</v>
+      </c>
+      <c r="S15" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1079,7 +1160,7 @@
         <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E16" t="s">
         <v>13</v>
@@ -1093,12 +1174,15 @@
       <c r="H16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1126,8 +1210,11 @@
       <c r="I18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -1135,7 +1222,7 @@
         <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E19" t="s">
         <v>12</v>
@@ -1149,8 +1236,11 @@
       <c r="H19" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
@@ -1158,7 +1248,7 @@
         <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E20" t="s">
         <v>13</v>
@@ -1172,12 +1262,15 @@
       <c r="H20" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -1206,7 +1299,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -1214,7 +1307,7 @@
         <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E23" t="s">
         <v>12</v>
@@ -1229,7 +1322,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -1237,7 +1330,7 @@
         <v>31</v>
       </c>
       <c r="D24" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E24" t="s">
         <v>13</v>
@@ -1252,11 +1345,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -1285,7 +1378,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -1293,7 +1386,7 @@
         <v>32</v>
       </c>
       <c r="D27" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E27" t="s">
         <v>12</v>
@@ -1308,7 +1401,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1316,7 +1409,7 @@
         <v>32</v>
       </c>
       <c r="D28" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E28" t="s">
         <v>13</v>
@@ -1331,11 +1424,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
@@ -1373,13 +1466,13 @@
         <v>5</v>
       </c>
       <c r="P30" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="Q30" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
@@ -1387,7 +1480,7 @@
         <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E31" t="s">
         <v>12</v>
@@ -1402,7 +1495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
@@ -1410,7 +1503,7 @@
         <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E32" t="s">
         <v>13</v>
@@ -1425,11 +1518,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
@@ -1458,7 +1551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
@@ -1466,7 +1559,7 @@
         <v>36</v>
       </c>
       <c r="D35" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
@@ -1481,7 +1574,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -1489,7 +1582,7 @@
         <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E36" t="s">
         <v>13</v>
@@ -1504,11 +1597,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
@@ -1537,7 +1630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
@@ -1545,7 +1638,7 @@
         <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -1560,7 +1653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>35</v>
       </c>
@@ -1568,7 +1661,7 @@
         <v>37</v>
       </c>
       <c r="D40" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E40" t="s">
         <v>13</v>
@@ -1583,11 +1676,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>57</v>
       </c>
@@ -1625,13 +1718,16 @@
         <v>5</v>
       </c>
       <c r="P42" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="Q42" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>57</v>
       </c>
@@ -1639,7 +1735,7 @@
         <v>39</v>
       </c>
       <c r="D43" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E43" t="s">
         <v>12</v>
@@ -1653,8 +1749,11 @@
       <c r="H43" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>57</v>
       </c>
@@ -1662,7 +1761,7 @@
         <v>39</v>
       </c>
       <c r="D44" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E44" t="s">
         <v>13</v>
@@ -1676,733 +1775,661 @@
       <c r="H44" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-    </row>
-    <row r="46" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="S46" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S47" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C46" t="b">
-        <v>1</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="C49" t="b">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
         <v>11</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E49" t="s">
         <v>53</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F49" t="s">
         <v>38</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G49" t="s">
         <v>15</v>
       </c>
-      <c r="H46" t="s">
-        <v>4</v>
-      </c>
-      <c r="I46">
-        <v>1</v>
-      </c>
-      <c r="J46" t="s">
+      <c r="H49" t="s">
+        <v>4</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49" t="s">
         <v>50</v>
       </c>
-      <c r="N46" t="s">
+      <c r="N49" t="s">
         <v>56</v>
       </c>
-      <c r="O46" t="s">
+      <c r="O49" t="s">
         <v>5</v>
       </c>
-      <c r="P46" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q46" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="P49" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q49" t="b">
+        <v>1</v>
+      </c>
+      <c r="S49" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D47" t="s">
-        <v>92</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="D50" t="s">
+        <v>86</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F47">
+      <c r="F50">
         <v>20000000</v>
       </c>
-      <c r="G47" t="s">
-        <v>9</v>
-      </c>
-      <c r="H47" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+      <c r="G50" t="s">
+        <v>9</v>
+      </c>
+      <c r="H50" t="s">
+        <v>4</v>
+      </c>
+      <c r="S50" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D48" t="s">
-        <v>92</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="D51" t="s">
+        <v>86</v>
+      </c>
+      <c r="E51" t="s">
         <v>13</v>
       </c>
-      <c r="F48">
+      <c r="F51">
         <v>0</v>
       </c>
-      <c r="G48" t="s">
-        <v>9</v>
-      </c>
-      <c r="H48" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+      <c r="G51" t="s">
+        <v>9</v>
+      </c>
+      <c r="H51" t="s">
+        <v>4</v>
+      </c>
+      <c r="S51" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S52" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S53" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E54" s="3"/>
+      <c r="S54" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C50" t="b">
-        <v>1</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="C56" t="b">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
         <v>11</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E56" t="s">
         <v>53</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F56" t="s">
         <v>38</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G56" t="s">
         <v>15</v>
       </c>
-      <c r="H50" t="s">
-        <v>4</v>
-      </c>
-      <c r="I50">
-        <v>1</v>
-      </c>
-      <c r="J50" t="s">
+      <c r="H56" t="s">
+        <v>4</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="J56" t="s">
         <v>50</v>
       </c>
-      <c r="N50" t="s">
+      <c r="N56" t="s">
         <v>56</v>
       </c>
-      <c r="O50" t="s">
+      <c r="O56" t="s">
         <v>5</v>
       </c>
-      <c r="P50" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q50" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+      <c r="P56" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D51" t="s">
-        <v>92</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="D57" t="s">
+        <v>86</v>
+      </c>
+      <c r="E57" t="s">
         <v>41</v>
       </c>
-      <c r="F51">
+      <c r="F57">
         <v>100000000</v>
       </c>
-      <c r="G51" t="s">
-        <v>9</v>
-      </c>
-      <c r="H51" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+      <c r="G57" t="s">
+        <v>9</v>
+      </c>
+      <c r="H57" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D52" t="s">
-        <v>92</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="D58" t="s">
+        <v>86</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F52">
+      <c r="F58">
         <v>20000000</v>
       </c>
-      <c r="G52" t="s">
-        <v>9</v>
-      </c>
-      <c r="H52" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+      <c r="G58" t="s">
+        <v>9</v>
+      </c>
+      <c r="H58" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C54" t="b">
-        <v>1</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="C60" t="b">
+        <v>1</v>
+      </c>
+      <c r="D60" t="s">
         <v>11</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E60" t="s">
         <v>53</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F60" t="s">
         <v>38</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G60" t="s">
         <v>15</v>
       </c>
-      <c r="H54" t="s">
-        <v>4</v>
-      </c>
-      <c r="I54">
-        <v>1</v>
-      </c>
-      <c r="J54" t="s">
+      <c r="H60" t="s">
+        <v>4</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60" t="s">
         <v>50</v>
       </c>
-      <c r="N54" t="s">
+      <c r="N60" t="s">
         <v>56</v>
       </c>
-      <c r="O54" t="s">
+      <c r="O60" t="s">
         <v>5</v>
       </c>
-      <c r="P54" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q54" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+      <c r="P60" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D55" t="s">
-        <v>92</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="D61" t="s">
+        <v>86</v>
+      </c>
+      <c r="E61" t="s">
         <v>41</v>
       </c>
-      <c r="F55">
+      <c r="F61">
         <v>100000000</v>
       </c>
-      <c r="G55" t="s">
-        <v>9</v>
-      </c>
-      <c r="H55" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+      <c r="G61" t="s">
+        <v>9</v>
+      </c>
+      <c r="H61" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D56" t="s">
-        <v>92</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="D62" t="s">
+        <v>86</v>
+      </c>
+      <c r="E62" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F56">
+      <c r="F62">
         <v>20000000</v>
       </c>
-      <c r="G56" t="s">
-        <v>9</v>
-      </c>
-      <c r="H56" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-    </row>
-    <row r="58" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+      <c r="G62" t="s">
+        <v>9</v>
+      </c>
+      <c r="H62" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C58" t="b">
-        <v>1</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="C64" t="b">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
         <v>11</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E64" t="s">
         <v>53</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F64" t="s">
         <v>27</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G64" t="s">
         <v>15</v>
       </c>
-      <c r="H58" t="s">
-        <v>4</v>
-      </c>
-      <c r="I58">
-        <v>1</v>
-      </c>
-      <c r="J58" t="s">
+      <c r="H64" t="s">
+        <v>4</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="J64" t="s">
         <v>50</v>
       </c>
-      <c r="N58" t="s">
+      <c r="N64" t="s">
         <v>56</v>
       </c>
-      <c r="O58" t="s">
+      <c r="O64" t="s">
         <v>5</v>
       </c>
-      <c r="P58" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q58" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+      <c r="P64" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q64" t="b">
+        <v>1</v>
+      </c>
+      <c r="S64" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D59" t="s">
-        <v>92</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="D65" t="s">
+        <v>86</v>
+      </c>
+      <c r="E65" t="s">
         <v>41</v>
       </c>
-      <c r="F59">
+      <c r="F65">
         <v>10000</v>
       </c>
-      <c r="G59" t="s">
-        <v>9</v>
-      </c>
-      <c r="H59" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+      <c r="G65" t="s">
+        <v>9</v>
+      </c>
+      <c r="H65" t="s">
+        <v>4</v>
+      </c>
+      <c r="S65" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D60" t="s">
-        <v>92</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="D66" t="s">
+        <v>86</v>
+      </c>
+      <c r="E66" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F60">
+      <c r="F66">
         <v>0</v>
       </c>
-      <c r="G60" t="s">
-        <v>9</v>
-      </c>
-      <c r="H60" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+      <c r="G66" t="s">
+        <v>9</v>
+      </c>
+      <c r="H66" t="s">
+        <v>4</v>
+      </c>
+      <c r="S66" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S67" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S68" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S69" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="E70" s="3"/>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C62" t="b">
-        <v>1</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="C71" t="b">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
         <v>11</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E71" t="s">
         <v>53</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F71" t="s">
         <v>27</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G71" t="s">
         <v>15</v>
       </c>
-      <c r="H62" t="s">
-        <v>4</v>
-      </c>
-      <c r="I62">
-        <v>1</v>
-      </c>
-      <c r="J62" t="s">
+      <c r="H71" t="s">
+        <v>4</v>
+      </c>
+      <c r="I71">
+        <v>1</v>
+      </c>
+      <c r="J71" t="s">
         <v>50</v>
       </c>
-      <c r="N62" t="s">
+      <c r="N71" t="s">
         <v>56</v>
       </c>
-      <c r="O62" t="s">
+      <c r="O71" t="s">
         <v>5</v>
       </c>
-      <c r="P62" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q62" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+      <c r="P71" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D63" t="s">
-        <v>92</v>
-      </c>
-      <c r="E63" t="s">
+      <c r="D72" t="s">
+        <v>86</v>
+      </c>
+      <c r="E72" t="s">
         <v>12</v>
       </c>
-      <c r="F63">
+      <c r="F72">
         <v>5000000</v>
       </c>
-      <c r="G63" t="s">
-        <v>9</v>
-      </c>
-      <c r="H63" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+      <c r="G72" t="s">
+        <v>9</v>
+      </c>
+      <c r="H72" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D64" t="s">
-        <v>92</v>
-      </c>
-      <c r="E64" t="s">
+      <c r="D73" t="s">
+        <v>86</v>
+      </c>
+      <c r="E73" t="s">
         <v>13</v>
       </c>
-      <c r="F64">
+      <c r="F73">
         <v>0</v>
       </c>
-      <c r="G64" t="s">
-        <v>9</v>
-      </c>
-      <c r="H64" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+      <c r="G73" t="s">
+        <v>9</v>
+      </c>
+      <c r="H73" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="E74" s="3"/>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C66" t="b">
-        <v>1</v>
-      </c>
-      <c r="D66" t="s">
-        <v>11</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F66" t="s">
-        <v>27</v>
-      </c>
-      <c r="G66" t="s">
-        <v>15</v>
-      </c>
-      <c r="H66" t="s">
-        <v>4</v>
-      </c>
-      <c r="I66">
-        <v>1</v>
-      </c>
-      <c r="J66" t="s">
-        <v>50</v>
-      </c>
-      <c r="N66" t="s">
-        <v>56</v>
-      </c>
-      <c r="O66" t="s">
-        <v>5</v>
-      </c>
-      <c r="P66" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q66" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D67" t="s">
-        <v>92</v>
-      </c>
-      <c r="E67" t="s">
-        <v>12</v>
-      </c>
-      <c r="F67">
-        <v>50000000</v>
-      </c>
-      <c r="G67" t="s">
-        <v>9</v>
-      </c>
-      <c r="H67" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D68" t="s">
-        <v>92</v>
-      </c>
-      <c r="E68" t="s">
-        <v>13</v>
-      </c>
-      <c r="F68">
-        <v>5000000</v>
-      </c>
-      <c r="G68" t="s">
-        <v>9</v>
-      </c>
-      <c r="H68" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C70" t="b">
-        <v>1</v>
-      </c>
-      <c r="D70" t="s">
-        <v>11</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F70" t="s">
-        <v>38</v>
-      </c>
-      <c r="G70" t="s">
-        <v>15</v>
-      </c>
-      <c r="H70" t="s">
-        <v>4</v>
-      </c>
-      <c r="I70">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D71" t="s">
-        <v>92</v>
-      </c>
-      <c r="E71" t="s">
-        <v>12</v>
-      </c>
-      <c r="F71">
-        <v>5000000</v>
-      </c>
-      <c r="G71" t="s">
-        <v>9</v>
-      </c>
-      <c r="H71" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D72" t="s">
-        <v>92</v>
-      </c>
-      <c r="E72" t="s">
-        <v>13</v>
-      </c>
-      <c r="F72">
-        <v>0</v>
-      </c>
-      <c r="G72" t="s">
-        <v>9</v>
-      </c>
-      <c r="H72" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C74" t="b">
-        <v>1</v>
-      </c>
-      <c r="D74" t="s">
-        <v>11</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F74" t="s">
-        <v>27</v>
-      </c>
-      <c r="G74" t="s">
-        <v>15</v>
-      </c>
-      <c r="H74" t="s">
-        <v>4</v>
-      </c>
-      <c r="I74">
-        <v>1</v>
-      </c>
-      <c r="J74" t="s">
-        <v>50</v>
-      </c>
-      <c r="N74" t="s">
-        <v>56</v>
-      </c>
-      <c r="O74" t="s">
-        <v>5</v>
-      </c>
-      <c r="P74" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q74" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="C75" t="b">
+        <v>1</v>
+      </c>
       <c r="D75" t="s">
-        <v>92</v>
+        <v>11</v>
       </c>
       <c r="E75" t="s">
-        <v>12</v>
-      </c>
-      <c r="F75">
-        <v>100000000</v>
+        <v>53</v>
+      </c>
+      <c r="F75" t="s">
+        <v>27</v>
       </c>
       <c r="G75" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H75" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I75">
+        <v>1</v>
+      </c>
+      <c r="J75" t="s">
+        <v>50</v>
+      </c>
+      <c r="N75" t="s">
+        <v>56</v>
+      </c>
+      <c r="O75" t="s">
+        <v>5</v>
+      </c>
+      <c r="P75" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D76" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E76" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F76">
         <v>50000000</v>
@@ -2414,73 +2441,75 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A77" s="1"/>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C78" t="b">
-        <v>1</v>
-      </c>
-      <c r="D78" t="s">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B77" t="s">
+        <v>72</v>
+      </c>
+      <c r="D77" t="s">
+        <v>86</v>
+      </c>
+      <c r="E77" t="s">
+        <v>13</v>
+      </c>
+      <c r="F77">
+        <v>5000000</v>
+      </c>
+      <c r="G77" t="s">
+        <v>9</v>
+      </c>
+      <c r="H77" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="E78" s="3"/>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C79" t="b">
+        <v>1</v>
+      </c>
+      <c r="D79" t="s">
         <v>11</v>
       </c>
-      <c r="E78" s="3" t="s">
+      <c r="E79" t="s">
         <v>53</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F79" t="s">
         <v>38</v>
       </c>
-      <c r="G78" t="s">
+      <c r="G79" t="s">
         <v>15</v>
       </c>
-      <c r="H78" t="s">
-        <v>4</v>
-      </c>
-      <c r="I78">
+      <c r="H79" t="s">
+        <v>4</v>
+      </c>
+      <c r="I79">
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D79" t="s">
-        <v>92</v>
-      </c>
-      <c r="E79" t="s">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D80" t="s">
+        <v>86</v>
+      </c>
+      <c r="E80" t="s">
         <v>12</v>
-      </c>
-      <c r="F79">
-        <v>50000000</v>
-      </c>
-      <c r="G79" t="s">
-        <v>9</v>
-      </c>
-      <c r="H79" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D80" t="s">
-        <v>92</v>
-      </c>
-      <c r="E80" t="s">
-        <v>13</v>
       </c>
       <c r="F80">
         <v>5000000</v>
@@ -2493,59 +2522,75 @@
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
+      <c r="A81" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D81" t="s">
+        <v>86</v>
+      </c>
+      <c r="E81" t="s">
+        <v>13</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81" t="s">
+        <v>9</v>
+      </c>
+      <c r="H81" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C82" t="b">
-        <v>1</v>
-      </c>
-      <c r="D82" t="s">
-        <v>11</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F82" t="s">
-        <v>38</v>
-      </c>
-      <c r="G82" t="s">
-        <v>15</v>
-      </c>
-      <c r="H82" t="s">
-        <v>4</v>
-      </c>
-      <c r="I82">
-        <v>3</v>
-      </c>
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="E82" s="3"/>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>74</v>
+        <v>112</v>
+      </c>
+      <c r="C83" t="b">
+        <v>1</v>
       </c>
       <c r="D83" t="s">
-        <v>92</v>
+        <v>11</v>
       </c>
       <c r="E83" t="s">
-        <v>12</v>
-      </c>
-      <c r="F83">
-        <v>100000000</v>
+        <v>53</v>
+      </c>
+      <c r="F83" t="s">
+        <v>27</v>
       </c>
       <c r="G83" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H83" t="s">
         <v>4</v>
+      </c>
+      <c r="I83">
+        <v>1</v>
+      </c>
+      <c r="J83" t="s">
+        <v>50</v>
+      </c>
+      <c r="N83" t="s">
+        <v>56</v>
+      </c>
+      <c r="O83" t="s">
+        <v>5</v>
+      </c>
+      <c r="P83" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q83" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.3">
@@ -2553,279 +2598,461 @@
         <v>49</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="D84" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E84" t="s">
+        <v>12</v>
+      </c>
+      <c r="F84">
+        <v>100000000</v>
+      </c>
+      <c r="G84" t="s">
+        <v>9</v>
+      </c>
+      <c r="H84" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D85" t="s">
+        <v>86</v>
+      </c>
+      <c r="E85" t="s">
         <v>13</v>
       </c>
-      <c r="F84">
+      <c r="F85">
         <v>50000000</v>
       </c>
-      <c r="G84" t="s">
-        <v>9</v>
-      </c>
-      <c r="H84" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
+      <c r="G85" t="s">
+        <v>9</v>
+      </c>
+      <c r="H85" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="86" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C86" t="b">
-        <v>1</v>
-      </c>
-      <c r="D86" t="s">
-        <v>17</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F86" t="s">
-        <v>62</v>
-      </c>
-      <c r="G86" t="s">
-        <v>15</v>
-      </c>
-      <c r="H86" t="s">
-        <v>4</v>
-      </c>
-      <c r="I86">
-        <v>1</v>
-      </c>
-      <c r="J86" t="s">
-        <v>50</v>
-      </c>
-      <c r="N86" t="s">
-        <v>56</v>
-      </c>
-      <c r="O86" t="s">
-        <v>5</v>
-      </c>
-      <c r="P86" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q86" t="b">
-        <v>1</v>
-      </c>
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="E86" s="3"/>
     </row>
     <row r="87" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>76</v>
+        <v>113</v>
+      </c>
+      <c r="C87" t="b">
+        <v>1</v>
       </c>
       <c r="D87" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="E87" t="s">
-        <v>13</v>
-      </c>
-      <c r="F87" s="4">
-        <v>0.6</v>
+        <v>53</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="G87" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="H87" t="s">
         <v>4</v>
       </c>
-      <c r="J87" t="s">
-        <v>5</v>
-      </c>
-      <c r="K87" t="s">
-        <v>69</v>
-      </c>
-      <c r="L87" t="s">
-        <v>68</v>
-      </c>
-      <c r="M87" t="b">
-        <v>1</v>
+      <c r="I87">
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="1"/>
-      <c r="E88" s="3"/>
+      <c r="A88" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D88" t="s">
+        <v>86</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F88">
+        <v>50000000</v>
+      </c>
+      <c r="G88" t="s">
+        <v>9</v>
+      </c>
+      <c r="H88" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="89" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C89" t="b">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="D89" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F89" t="s">
-        <v>65</v>
+        <v>13</v>
+      </c>
+      <c r="F89">
+        <v>5000000</v>
       </c>
       <c r="G89" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="H89" t="s">
         <v>4</v>
       </c>
-      <c r="I89">
-        <v>1</v>
-      </c>
-      <c r="J89" t="s">
-        <v>50</v>
-      </c>
-      <c r="N89" t="s">
-        <v>56</v>
-      </c>
-      <c r="O89" t="s">
-        <v>5</v>
-      </c>
-      <c r="P89" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q89" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D90" t="s">
-        <v>64</v>
-      </c>
-      <c r="E90" t="s">
-        <v>12</v>
-      </c>
-      <c r="F90" t="s">
-        <v>66</v>
-      </c>
-      <c r="G90" t="s">
-        <v>15</v>
-      </c>
-      <c r="H90" t="s">
-        <v>67</v>
-      </c>
-      <c r="J90" t="s">
-        <v>5</v>
-      </c>
-      <c r="K90" t="s">
-        <v>69</v>
-      </c>
-      <c r="L90" t="s">
-        <v>68</v>
-      </c>
-      <c r="M90" t="b">
-        <v>1</v>
-      </c>
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>77</v>
+        <v>114</v>
+      </c>
+      <c r="C91" t="b">
+        <v>1</v>
       </c>
       <c r="D91" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="E91" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="F91" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="G91" t="s">
         <v>15</v>
       </c>
       <c r="H91" t="s">
-        <v>67</v>
+        <v>4</v>
+      </c>
+      <c r="I91">
+        <v>3</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
       <c r="D92" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="E92" t="s">
         <v>12</v>
       </c>
-      <c r="F92" t="s">
-        <v>47</v>
+      <c r="F92">
+        <v>100000000</v>
       </c>
       <c r="G92" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="H92" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D93" t="s">
+        <v>86</v>
+      </c>
+      <c r="E93" t="s">
+        <v>13</v>
+      </c>
+      <c r="F93">
+        <v>50000000</v>
+      </c>
+      <c r="G93" t="s">
+        <v>9</v>
+      </c>
+      <c r="H93" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C95" t="b">
+        <v>1</v>
+      </c>
+      <c r="D95" t="s">
+        <v>17</v>
+      </c>
+      <c r="E95" t="s">
+        <v>53</v>
+      </c>
+      <c r="F95" t="s">
+        <v>62</v>
+      </c>
+      <c r="G95" t="s">
+        <v>15</v>
+      </c>
+      <c r="H95" t="s">
+        <v>4</v>
+      </c>
+      <c r="I95">
+        <v>1</v>
+      </c>
+      <c r="J95" t="s">
+        <v>50</v>
+      </c>
+      <c r="N95" t="s">
+        <v>56</v>
+      </c>
+      <c r="O95" t="s">
+        <v>5</v>
+      </c>
+      <c r="P95" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q95" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D96" t="s">
+        <v>61</v>
+      </c>
+      <c r="E96" t="s">
+        <v>13</v>
+      </c>
+      <c r="F96" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="G96" t="s">
+        <v>63</v>
+      </c>
+      <c r="H96" t="s">
+        <v>4</v>
+      </c>
+      <c r="J96" t="s">
+        <v>5</v>
+      </c>
+      <c r="K96" t="s">
+        <v>69</v>
+      </c>
+      <c r="L96" t="s">
+        <v>68</v>
+      </c>
+      <c r="M96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" spans="1:17" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="B98" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C98" t="b">
+        <v>1</v>
+      </c>
+      <c r="D98" t="s">
+        <v>17</v>
+      </c>
+      <c r="E98" t="s">
+        <v>53</v>
+      </c>
+      <c r="F98" t="s">
+        <v>65</v>
+      </c>
+      <c r="G98" t="s">
+        <v>15</v>
+      </c>
+      <c r="H98" t="s">
+        <v>4</v>
+      </c>
+      <c r="I98">
+        <v>1</v>
+      </c>
+      <c r="J98" t="s">
+        <v>50</v>
+      </c>
+      <c r="N98" t="s">
+        <v>56</v>
+      </c>
+      <c r="O98" t="s">
+        <v>5</v>
+      </c>
+      <c r="P98" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q98" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D99" t="s">
         <v>64</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E99" t="s">
         <v>12</v>
       </c>
-      <c r="F93" t="s">
+      <c r="F99" t="s">
+        <v>66</v>
+      </c>
+      <c r="G99" t="s">
+        <v>15</v>
+      </c>
+      <c r="H99" t="s">
+        <v>67</v>
+      </c>
+      <c r="J99" t="s">
+        <v>5</v>
+      </c>
+      <c r="K99" t="s">
+        <v>69</v>
+      </c>
+      <c r="L99" t="s">
+        <v>68</v>
+      </c>
+      <c r="M99" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D100" t="s">
+        <v>64</v>
+      </c>
+      <c r="E100" t="s">
+        <v>12</v>
+      </c>
+      <c r="F100" t="s">
+        <v>71</v>
+      </c>
+      <c r="G100" t="s">
+        <v>15</v>
+      </c>
+      <c r="H100" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D101" t="s">
+        <v>64</v>
+      </c>
+      <c r="E101" t="s">
+        <v>12</v>
+      </c>
+      <c r="F101" t="s">
+        <v>47</v>
+      </c>
+      <c r="G101" t="s">
+        <v>15</v>
+      </c>
+      <c r="H101" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D102" t="s">
+        <v>64</v>
+      </c>
+      <c r="E102" t="s">
+        <v>12</v>
+      </c>
+      <c r="F102" t="s">
         <v>48</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G102" t="s">
         <v>15</v>
       </c>
-      <c r="H93" t="s">
+      <c r="H102" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A94" s="1" t="s">
+    <row r="103" spans="1:17" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B94" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="B103" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D103" t="s">
         <v>64</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E103" t="s">
         <v>12</v>
       </c>
-      <c r="F94" t="s">
+      <c r="F103" t="s">
         <v>49</v>
       </c>
-      <c r="G94" t="s">
+      <c r="G103" t="s">
         <v>15</v>
       </c>
-      <c r="H94" t="s">
+      <c r="H103" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix(infrastructure): rule seed reasons for msme
</commit_message>
<xml_diff>
--- a/apps/server/infrastructure-be/src/modules/seeders/seedData.xlsx
+++ b/apps/server/infrastructure-be/src/modules/seeders/seedData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="144">
   <si>
     <t xml:space="preserve">ruleDesigner</t>
   </si>
@@ -300,6 +300,18 @@
     <t xml:space="preserve">Rule sixteen</t>
   </si>
   <si>
+    <t xml:space="preserve">Changes in legal regulatory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diversification of Suppliers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limited Supplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Market Dynamics:</t>
+  </si>
+  <si>
     <t xml:space="preserve">Small</t>
   </si>
   <si>
@@ -309,13 +321,13 @@
     <t xml:space="preserve">Rule eighteen</t>
   </si>
   <si>
+    <t xml:space="preserve">Rule twenty</t>
+  </si>
+  <si>
     <t xml:space="preserve">Medium</t>
   </si>
   <si>
     <t xml:space="preserve">Rule nineteen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rule twenty</t>
   </si>
   <si>
     <t xml:space="preserve">Rule twentyone</t>
@@ -549,6 +561,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -557,15 +573,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -761,10 +773,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S159"/>
+  <dimension ref="A1:S1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F136" activeCellId="0" sqref="F136"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C64" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S88" activeCellId="0" sqref="S88:S90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2388,6 +2400,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="S71" s="5" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
@@ -2411,6 +2426,9 @@
       <c r="H72" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="S72" s="5" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
@@ -2434,271 +2452,262 @@
       <c r="H73" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="S73" s="5" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="2"/>
-      <c r="B74" s="2"/>
+      <c r="A74" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D74" s="4"/>
       <c r="E74" s="4"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="4"/>
+      <c r="S74" s="5" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C75" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F75" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G75" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H75" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I75" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J75" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="N75" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="O75" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P75" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q75" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="E75" s="4"/>
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C76" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I76" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J76" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N76" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O76" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P76" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q76" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="S76" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E76" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F76" s="1" t="n">
-        <v>50000000</v>
-      </c>
-      <c r="G76" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H76" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E77" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F77" s="1" t="n">
+        <v>50000000</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="S77" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E78" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F77" s="1" t="n">
+      <c r="F78" s="1" t="n">
         <v>5000000</v>
       </c>
-      <c r="G77" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H77" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="2"/>
-      <c r="B78" s="2"/>
-      <c r="E78" s="4"/>
+      <c r="G78" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="S78" s="5" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C79" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E79" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F79" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G79" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H79" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I79" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
+      <c r="E79" s="4"/>
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
+      </c>
+      <c r="C80" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F80" s="1" t="n">
-        <v>5000000</v>
+        <v>22</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="H80" s="4" t="s">
         <v>25</v>
+      </c>
+      <c r="I80" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S80" s="5" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E81" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F81" s="1" t="n">
+        <v>5000000</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E82" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F81" s="1" t="n">
+      <c r="F82" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G81" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H81" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="2"/>
-      <c r="B82" s="2"/>
-      <c r="E82" s="4"/>
+      <c r="G82" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B83" s="2" t="s">
+      <c r="A83" s="2"/>
+      <c r="B83" s="2"/>
+      <c r="E83" s="4"/>
+    </row>
+    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C83" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D83" s="4" t="s">
+      <c r="B84" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C84" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D84" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E83" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F83" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G83" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H83" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I83" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J83" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="N83" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="O83" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P83" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q83" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B84" s="2" t="s">
+      <c r="E84" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H84" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I84" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D84" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F84" s="1" t="n">
-        <v>100000000</v>
-      </c>
-      <c r="G84" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H84" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="B85" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F85" s="1" t="n">
         <v>50000000</v>
@@ -2710,1733 +2719,1800 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="2"/>
-      <c r="B86" s="2"/>
-      <c r="E86" s="4"/>
-    </row>
-    <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="2" t="s">
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F86" s="1" t="n">
+        <v>5000000</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2"/>
+      <c r="E87" s="4"/>
+    </row>
+    <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C88" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I88" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J88" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N88" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O88" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P88" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q88" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="S88" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B87" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C87" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D87" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E87" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G87" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H87" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I87" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D88" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E88" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F88" s="1" t="n">
-        <v>50000000</v>
-      </c>
-      <c r="G88" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H88" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E89" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F89" s="1" t="n">
+        <v>100000000</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="S89" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E90" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F89" s="1" t="n">
-        <v>5000000</v>
-      </c>
-      <c r="G89" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H89" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="2"/>
-      <c r="B90" s="2"/>
+      <c r="F90" s="1" t="n">
+        <v>50000000</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="S90" s="5" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C91" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D91" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E91" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F91" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G91" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H91" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I91" s="1" t="n">
-        <v>3</v>
-      </c>
+      <c r="A91" s="2"/>
+      <c r="B91" s="2"/>
     </row>
     <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C92" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H92" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I92" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="S92" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E92" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F92" s="1" t="n">
-        <v>100000000</v>
-      </c>
-      <c r="G92" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H92" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E93" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F93" s="1" t="n">
+        <v>100000000</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H93" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E94" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F93" s="1" t="n">
+      <c r="F94" s="1" t="n">
         <v>50000000</v>
       </c>
-      <c r="G93" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H93" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="2"/>
-      <c r="B94" s="2"/>
+      <c r="G94" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C95" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D95" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E95" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F95" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G95" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H95" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I95" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J95" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="N95" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="O95" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P95" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q95" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="A95" s="2"/>
+      <c r="B95" s="2"/>
     </row>
     <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
+      </c>
+      <c r="C96" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="D96" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G96" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H96" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I96" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J96" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N96" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O96" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P96" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q96" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E96" s="4" t="s">
+      <c r="B97" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E97" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F96" s="5" t="n">
+      <c r="F97" s="6" t="n">
         <v>0.6</v>
       </c>
-      <c r="G96" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="H96" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J96" s="4" t="s">
+      <c r="G97" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H97" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J97" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K96" s="4" t="s">
+      <c r="K97" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="L97" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="M97" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="2"/>
+      <c r="B98" s="2"/>
+    </row>
+    <row r="99" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A99" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C99" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D99" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="L96" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="M96" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="2"/>
-      <c r="B97" s="2"/>
-    </row>
-    <row r="98" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B98" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C98" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D98" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E98" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F98" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G98" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H98" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I98" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J98" s="4" t="s">
+      <c r="E99" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G99" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H99" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I99" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J99" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N98" s="4" t="s">
+      <c r="N99" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="O98" s="4" t="s">
+      <c r="O99" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="P98" s="4" t="s">
+      <c r="P99" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="Q98" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A99" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B99" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D99" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E99" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F99" s="4" t="s">
+      <c r="Q99" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A100" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G99" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H99" s="4" t="s">
+      <c r="B100" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="J99" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K99" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="L99" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="M99" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B100" s="6" t="s">
-        <v>108</v>
-      </c>
       <c r="D100" s="4" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E100" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G100" s="4" t="s">
         <v>24</v>
       </c>
       <c r="H100" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J100" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K100" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="L100" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="M100" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A101" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B101" s="7" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="101" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>108</v>
-      </c>
       <c r="D101" s="4" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E101" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="G101" s="4" t="s">
         <v>24</v>
       </c>
       <c r="H101" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A102" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B102" s="7" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="102" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>108</v>
-      </c>
       <c r="D102" s="4" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E102" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G102" s="4" t="s">
         <v>24</v>
       </c>
       <c r="H102" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A103" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B103" s="7" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B103" s="6" t="s">
-        <v>108</v>
-      </c>
       <c r="D103" s="4" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G103" s="4" t="s">
         <v>24</v>
       </c>
       <c r="H103" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A104" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B104" s="7" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="7" t="s">
+      <c r="D104" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B105" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="C105" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D105" s="7" t="s">
+      <c r="E104" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G104" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H104" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C106" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D106" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E105" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F105" s="7" t="s">
+      <c r="E106" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F106" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G105" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H105" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I105" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J105" s="7" t="s">
+      <c r="G106" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H106" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I106" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J106" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="N105" s="4" t="s">
+      <c r="N106" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B106" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="C106" s="8"/>
-      <c r="D106" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E106" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F106" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="G106" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H106" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I106" s="8"/>
-      <c r="J106" s="8"/>
-    </row>
     <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B107" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="C107" s="8"/>
-      <c r="D107" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E107" s="7" t="s">
+      <c r="A107" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C107" s="4"/>
+      <c r="D107" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E107" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F107" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G107" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H107" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I107" s="4"/>
+      <c r="J107" s="4"/>
+    </row>
+    <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C108" s="4"/>
+      <c r="D108" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E108" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F107" s="7" t="n">
+      <c r="F108" s="8" t="n">
         <v>100000000</v>
       </c>
-      <c r="G107" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H107" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I107" s="8"/>
-      <c r="J107" s="8"/>
-    </row>
-    <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="8"/>
-      <c r="B108" s="8"/>
-      <c r="C108" s="8"/>
-      <c r="D108" s="8"/>
-      <c r="E108" s="8"/>
-      <c r="F108" s="8"/>
-      <c r="G108" s="8"/>
-      <c r="H108" s="8"/>
-      <c r="I108" s="8"/>
-      <c r="J108" s="8"/>
+      <c r="G108" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H108" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I108" s="4"/>
+      <c r="J108" s="4"/>
     </row>
     <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B109" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C109" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D109" s="7" t="s">
+      <c r="A109" s="4"/>
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4"/>
+      <c r="G109" s="4"/>
+      <c r="H109" s="4"/>
+      <c r="I109" s="4"/>
+      <c r="J109" s="4"/>
+    </row>
+    <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C110" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D110" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E109" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F109" s="7" t="s">
+      <c r="E110" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F110" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G109" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H109" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I109" s="7" t="n">
+      <c r="G110" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H110" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I110" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="J109" s="8"/>
-    </row>
-    <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B110" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C110" s="8"/>
-      <c r="D110" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E110" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F110" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="G110" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H110" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I110" s="8"/>
-      <c r="J110" s="8"/>
+      <c r="J110" s="4"/>
     </row>
     <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B111" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C111" s="8"/>
-      <c r="D111" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E111" s="7" t="s">
+      <c r="A111" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B111" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C111" s="4"/>
+      <c r="D111" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E111" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F111" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G111" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H111" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I111" s="4"/>
+      <c r="J111" s="4"/>
+    </row>
+    <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B112" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C112" s="4"/>
+      <c r="D112" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E112" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F111" s="7" t="n">
+      <c r="F112" s="8" t="n">
         <v>150000000</v>
       </c>
-      <c r="G111" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H111" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I111" s="8"/>
-      <c r="J111" s="8"/>
-    </row>
-    <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="8"/>
-      <c r="B112" s="8"/>
-      <c r="C112" s="0"/>
-      <c r="D112" s="8"/>
-      <c r="E112" s="8"/>
-      <c r="F112" s="8"/>
-      <c r="G112" s="8"/>
-      <c r="H112" s="8"/>
-      <c r="I112" s="8"/>
-      <c r="J112" s="8"/>
+      <c r="G112" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H112" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I112" s="4"/>
+      <c r="J112" s="4"/>
     </row>
     <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B113" s="7" t="s">
+      <c r="A113" s="4"/>
+      <c r="B113" s="4"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="4"/>
+      <c r="G113" s="4"/>
+      <c r="H113" s="4"/>
+      <c r="I113" s="4"/>
+      <c r="J113" s="4"/>
+    </row>
+    <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="C113" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D113" s="7" t="s">
+      <c r="B114" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C114" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D114" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E113" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F113" s="5" t="s">
+      <c r="E114" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F114" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G113" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H113" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I113" s="7" t="n">
+      <c r="G114" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H114" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I114" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="J113" s="8"/>
-    </row>
-    <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B114" s="7" t="s">
+      <c r="J114" s="4"/>
+    </row>
+    <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="C114" s="8"/>
-      <c r="D114" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E114" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F114" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="G114" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H114" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I114" s="8"/>
-      <c r="J114" s="8"/>
-    </row>
-    <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B115" s="7" t="s">
+      <c r="B115" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C115" s="4"/>
+      <c r="D115" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E115" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F115" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G115" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H115" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I115" s="4"/>
+      <c r="J115" s="4"/>
+    </row>
+    <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="C115" s="8"/>
-      <c r="D115" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E115" s="7" t="s">
+      <c r="B116" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C116" s="4"/>
+      <c r="D116" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E116" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F115" s="7" t="n">
+      <c r="F116" s="8" t="n">
         <v>50000000</v>
       </c>
-      <c r="G115" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H115" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I115" s="8"/>
-      <c r="J115" s="8"/>
-    </row>
-    <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="8"/>
-      <c r="B116" s="8"/>
-      <c r="C116" s="8"/>
-      <c r="D116" s="8"/>
-      <c r="E116" s="8"/>
-      <c r="F116" s="8"/>
-      <c r="G116" s="8"/>
-      <c r="H116" s="8"/>
-      <c r="I116" s="8"/>
-      <c r="J116" s="8"/>
+      <c r="G116" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H116" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I116" s="4"/>
+      <c r="J116" s="4"/>
     </row>
     <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B117" s="7" t="s">
+      <c r="A117" s="4"/>
+      <c r="B117" s="4"/>
+      <c r="C117" s="4"/>
+      <c r="D117" s="4"/>
+      <c r="E117" s="4"/>
+      <c r="F117" s="4"/>
+      <c r="G117" s="4"/>
+      <c r="H117" s="4"/>
+      <c r="I117" s="4"/>
+      <c r="J117" s="4"/>
+    </row>
+    <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B118" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C118" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D118" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E118" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F118" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G118" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H118" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I118" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="J118" s="4"/>
+    </row>
+    <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C119" s="4"/>
+      <c r="D119" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E119" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F119" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G119" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H119" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I119" s="4"/>
+      <c r="J119" s="4"/>
+    </row>
+    <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C120" s="4"/>
+      <c r="D120" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="C117" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D117" s="7" t="s">
+      <c r="E120" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F120" s="8" t="n">
+        <v>100000000</v>
+      </c>
+      <c r="G120" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H120" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I120" s="4"/>
+      <c r="J120" s="4"/>
+    </row>
+    <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="4"/>
+      <c r="B121" s="4"/>
+      <c r="C121" s="4"/>
+      <c r="D121" s="4"/>
+      <c r="E121" s="4"/>
+      <c r="F121" s="4"/>
+      <c r="G121" s="4"/>
+      <c r="H121" s="4"/>
+      <c r="I121" s="4"/>
+      <c r="J121" s="4"/>
+    </row>
+    <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C122" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D122" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E117" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F117" s="5" t="s">
+      <c r="E122" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F122" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G122" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H122" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I122" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="J122" s="4"/>
+    </row>
+    <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C123" s="4"/>
+      <c r="D123" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E123" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F123" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G123" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H123" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I123" s="4"/>
+      <c r="J123" s="4"/>
+    </row>
+    <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C124" s="4"/>
+      <c r="D124" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E124" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F124" s="8" t="n">
+        <v>100000000</v>
+      </c>
+      <c r="G124" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H124" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I124" s="4"/>
+      <c r="J124" s="4"/>
+    </row>
+    <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="4"/>
+      <c r="B125" s="4"/>
+      <c r="C125" s="4"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="4"/>
+      <c r="F125" s="4"/>
+      <c r="G125" s="4"/>
+      <c r="H125" s="4"/>
+      <c r="I125" s="4"/>
+      <c r="J125" s="4"/>
+    </row>
+    <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C126" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D126" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E126" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F126" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G126" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H126" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I126" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="J126" s="4"/>
+    </row>
+    <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B127" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C127" s="4"/>
+      <c r="D127" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E127" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F127" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G127" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H127" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I127" s="4"/>
+      <c r="J127" s="4"/>
+    </row>
+    <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C128" s="4"/>
+      <c r="D128" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E128" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F128" s="8" t="n">
+        <v>5000000</v>
+      </c>
+      <c r="G128" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H128" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I128" s="4"/>
+      <c r="J128" s="4"/>
+    </row>
+    <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="4"/>
+      <c r="B129" s="4"/>
+      <c r="C129" s="4"/>
+      <c r="D129" s="4"/>
+      <c r="E129" s="4"/>
+      <c r="F129" s="4"/>
+      <c r="G129" s="4"/>
+      <c r="H129" s="4"/>
+      <c r="I129" s="4"/>
+      <c r="J129" s="4"/>
+    </row>
+    <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B130" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C130" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D130" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E130" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F130" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G130" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H130" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I130" s="8" t="n">
+        <v>7</v>
+      </c>
+      <c r="J130" s="4"/>
+    </row>
+    <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B131" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C131" s="4"/>
+      <c r="D131" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E131" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F131" s="8" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G131" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H131" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I131" s="4"/>
+      <c r="J131" s="4"/>
+    </row>
+    <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="4"/>
+      <c r="B132" s="4"/>
+      <c r="C132" s="4"/>
+      <c r="D132" s="4"/>
+      <c r="E132" s="4"/>
+      <c r="F132" s="4"/>
+      <c r="G132" s="4"/>
+      <c r="H132" s="4"/>
+      <c r="I132" s="4"/>
+      <c r="J132" s="4"/>
+    </row>
+    <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C133" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D133" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E133" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F133" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G133" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H133" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I133" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J133" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N133" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B134" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C134" s="4"/>
+      <c r="D134" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E134" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F134" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G134" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H134" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I134" s="4"/>
+      <c r="J134" s="4"/>
+    </row>
+    <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B135" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C135" s="4"/>
+      <c r="D135" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E135" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F135" s="8" t="n">
+        <v>5000000</v>
+      </c>
+      <c r="G135" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H135" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I135" s="4"/>
+      <c r="J135" s="4"/>
+    </row>
+    <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="4"/>
+      <c r="B136" s="4"/>
+      <c r="C136" s="4"/>
+      <c r="D136" s="4"/>
+      <c r="E136" s="4"/>
+      <c r="F136" s="4"/>
+      <c r="G136" s="4"/>
+      <c r="H136" s="4"/>
+      <c r="I136" s="4"/>
+      <c r="J136" s="4"/>
+    </row>
+    <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B137" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C137" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D137" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E137" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F137" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G117" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H117" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I117" s="7" t="n">
+      <c r="G137" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H137" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I137" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="J137" s="4"/>
+    </row>
+    <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B138" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C138" s="4"/>
+      <c r="D138" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E138" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F138" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G138" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H138" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I138" s="4"/>
+      <c r="J138" s="4"/>
+    </row>
+    <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C139" s="4"/>
+      <c r="D139" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E139" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F139" s="8" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="G139" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H139" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I139" s="4"/>
+      <c r="J139" s="4"/>
+    </row>
+    <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="4"/>
+      <c r="B140" s="4"/>
+      <c r="C140" s="4"/>
+      <c r="D140" s="4"/>
+      <c r="E140" s="4"/>
+      <c r="F140" s="4"/>
+      <c r="G140" s="4"/>
+      <c r="H140" s="4"/>
+      <c r="I140" s="4"/>
+      <c r="J140" s="4"/>
+    </row>
+    <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B141" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C141" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D141" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E141" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F141" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G141" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H141" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I141" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="J141" s="4"/>
+    </row>
+    <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B142" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C142" s="4"/>
+      <c r="D142" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E142" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F142" s="8" t="n">
+        <v>1500000000</v>
+      </c>
+      <c r="G142" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H142" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I142" s="4"/>
+      <c r="J142" s="4"/>
+    </row>
+    <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="4"/>
+      <c r="B143" s="4"/>
+      <c r="C143" s="4"/>
+      <c r="D143" s="4"/>
+      <c r="E143" s="4"/>
+      <c r="F143" s="4"/>
+      <c r="G143" s="4"/>
+      <c r="H143" s="4"/>
+      <c r="I143" s="4"/>
+      <c r="J143" s="4"/>
+    </row>
+    <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B144" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C144" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D144" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E144" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F144" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G144" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H144" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I144" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="J117" s="8"/>
-    </row>
-    <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B118" s="7" t="s">
+      <c r="J144" s="4"/>
+    </row>
+    <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B145" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C145" s="4"/>
+      <c r="D145" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="C118" s="8"/>
-      <c r="D118" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E118" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F118" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G118" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H118" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I118" s="8"/>
-      <c r="J118" s="8"/>
-    </row>
-    <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B119" s="7" t="s">
+      <c r="E145" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F145" s="8" t="n">
+        <v>3500000000</v>
+      </c>
+      <c r="G145" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H145" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I145" s="4"/>
+      <c r="J145" s="4"/>
+    </row>
+    <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="4"/>
+      <c r="B146" s="4"/>
+      <c r="C146" s="4"/>
+      <c r="D146" s="4"/>
+      <c r="E146" s="4"/>
+      <c r="F146" s="4"/>
+      <c r="G146" s="4"/>
+      <c r="H146" s="4"/>
+      <c r="I146" s="4"/>
+      <c r="J146" s="4"/>
+    </row>
+    <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B147" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C147" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D147" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E147" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F147" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G147" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H147" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I147" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="J147" s="4"/>
+    </row>
+    <row r="148" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B148" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C148" s="4"/>
+      <c r="D148" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="C119" s="8"/>
-      <c r="D119" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E119" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F119" s="7" t="n">
-        <v>100000000</v>
-      </c>
-      <c r="G119" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H119" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I119" s="8"/>
-      <c r="J119" s="8"/>
-    </row>
-    <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="8"/>
-      <c r="B120" s="8"/>
-      <c r="C120" s="8"/>
-      <c r="D120" s="8"/>
-      <c r="E120" s="8"/>
-      <c r="F120" s="8"/>
-      <c r="G120" s="8"/>
-      <c r="H120" s="8"/>
-      <c r="I120" s="8"/>
-      <c r="J120" s="8"/>
-    </row>
-    <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B121" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="C121" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D121" s="7" t="s">
+      <c r="E148" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F148" s="8" t="n">
+        <v>1500000000</v>
+      </c>
+      <c r="G148" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H148" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I148" s="4"/>
+      <c r="J148" s="4"/>
+    </row>
+    <row r="149" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="4"/>
+      <c r="B149" s="4"/>
+      <c r="C149" s="4"/>
+      <c r="D149" s="4"/>
+      <c r="E149" s="4"/>
+      <c r="F149" s="4"/>
+      <c r="G149" s="4"/>
+      <c r="H149" s="4"/>
+      <c r="I149" s="4"/>
+      <c r="J149" s="4"/>
+    </row>
+    <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B150" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C150" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D150" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E121" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F121" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G121" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H121" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I121" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="J121" s="8"/>
-    </row>
-    <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B122" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="C122" s="8"/>
-      <c r="D122" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E122" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F122" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="G122" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H122" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I122" s="8"/>
-      <c r="J122" s="8"/>
-    </row>
-    <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B123" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="C123" s="8"/>
-      <c r="D123" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E123" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F123" s="7" t="n">
-        <v>100000000</v>
-      </c>
-      <c r="G123" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H123" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I123" s="8"/>
-      <c r="J123" s="8"/>
-    </row>
-    <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="8"/>
-      <c r="B124" s="8"/>
-      <c r="C124" s="8"/>
-      <c r="D124" s="8"/>
-      <c r="E124" s="8"/>
-      <c r="F124" s="8"/>
-      <c r="G124" s="8"/>
-      <c r="H124" s="8"/>
-      <c r="I124" s="8"/>
-      <c r="J124" s="8"/>
-    </row>
-    <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B125" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C125" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D125" s="7" t="s">
+      <c r="E150" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F150" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G150" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H150" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I150" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J150" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N150" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B151" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C151" s="4"/>
+      <c r="D151" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E151" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F151" s="8" t="n">
+        <v>1500000000</v>
+      </c>
+      <c r="G151" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H151" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I151" s="4"/>
+      <c r="J151" s="4"/>
+    </row>
+    <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="4"/>
+      <c r="B152" s="4"/>
+      <c r="C152" s="4"/>
+      <c r="D152" s="4"/>
+      <c r="E152" s="4"/>
+      <c r="F152" s="4"/>
+      <c r="G152" s="4"/>
+      <c r="H152" s="4"/>
+      <c r="I152" s="4"/>
+      <c r="J152" s="4"/>
+    </row>
+    <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B153" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C153" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D153" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E125" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F125" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="G125" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H125" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I125" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="J125" s="8"/>
-    </row>
-    <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B126" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C126" s="8"/>
-      <c r="D126" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E126" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F126" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="G126" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H126" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I126" s="8"/>
-      <c r="J126" s="8"/>
-    </row>
-    <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B127" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C127" s="8"/>
-      <c r="D127" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E127" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F127" s="7" t="n">
-        <v>5000000</v>
-      </c>
-      <c r="G127" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H127" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I127" s="8"/>
-      <c r="J127" s="8"/>
-    </row>
-    <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="8"/>
-      <c r="B128" s="8"/>
-      <c r="C128" s="8"/>
-      <c r="D128" s="8"/>
-      <c r="E128" s="8"/>
-      <c r="F128" s="8"/>
-      <c r="G128" s="8"/>
-      <c r="H128" s="8"/>
-      <c r="I128" s="8"/>
-      <c r="J128" s="8"/>
-    </row>
-    <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B129" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C129" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D129" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E129" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F129" s="7" t="s">
+      <c r="E153" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F153" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G153" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H153" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I153" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="J153" s="4"/>
+    </row>
+    <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B154" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C154" s="4"/>
+      <c r="D154" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E154" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F154" s="8" t="n">
+        <v>3500000000</v>
+      </c>
+      <c r="G154" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H154" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I154" s="4"/>
+      <c r="J154" s="4"/>
+    </row>
+    <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="4"/>
+      <c r="B155" s="4"/>
+      <c r="C155" s="4"/>
+      <c r="D155" s="4"/>
+      <c r="E155" s="4"/>
+      <c r="F155" s="4"/>
+      <c r="G155" s="4"/>
+      <c r="H155" s="4"/>
+      <c r="I155" s="4"/>
+      <c r="J155" s="4"/>
+    </row>
+    <row r="156" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C156" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D156" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E156" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F156" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G156" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H156" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I156" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="J156" s="4"/>
+    </row>
+    <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B157" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C157" s="4"/>
+      <c r="D157" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E157" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F157" s="8" t="n">
+        <v>1500000000</v>
+      </c>
+      <c r="G157" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H157" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I157" s="4"/>
+      <c r="J157" s="4"/>
+    </row>
+    <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="4"/>
+      <c r="B158" s="4"/>
+      <c r="C158" s="4"/>
+      <c r="D158" s="4"/>
+      <c r="E158" s="4"/>
+      <c r="F158" s="4"/>
+      <c r="G158" s="4"/>
+      <c r="H158" s="4"/>
+      <c r="I158" s="4"/>
+      <c r="J158" s="4"/>
+    </row>
+    <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C159" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D159" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E159" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F159" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G129" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H129" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I129" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="J129" s="8"/>
-    </row>
-    <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B130" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C130" s="8"/>
-      <c r="D130" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E130" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F130" s="7" t="n">
+      <c r="G159" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H159" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I159" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="J159" s="4"/>
+    </row>
+    <row r="160" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B160" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C160" s="4"/>
+      <c r="D160" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E160" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F160" s="8" t="n">
         <v>10000</v>
       </c>
-      <c r="G130" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H130" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I130" s="8"/>
-      <c r="J130" s="8"/>
-    </row>
-    <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="8"/>
-      <c r="B131" s="8"/>
-      <c r="C131" s="8"/>
-      <c r="D131" s="8"/>
-      <c r="E131" s="8"/>
-      <c r="F131" s="8"/>
-      <c r="G131" s="8"/>
-      <c r="H131" s="8"/>
-      <c r="I131" s="8"/>
-      <c r="J131" s="8"/>
-    </row>
-    <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B132" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C132" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D132" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E132" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F132" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="G132" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H132" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I132" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J132" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="N132" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B133" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C133" s="8"/>
-      <c r="D133" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E133" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F133" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="G133" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H133" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I133" s="8"/>
-      <c r="J133" s="8"/>
-    </row>
-    <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B134" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C134" s="8"/>
-      <c r="D134" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E134" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F134" s="7" t="n">
-        <v>5000000</v>
-      </c>
-      <c r="G134" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H134" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I134" s="8"/>
-      <c r="J134" s="8"/>
-    </row>
-    <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="8"/>
-      <c r="B135" s="8"/>
-      <c r="C135" s="8"/>
-      <c r="D135" s="8"/>
-      <c r="E135" s="8"/>
-      <c r="F135" s="8"/>
-      <c r="G135" s="8"/>
-      <c r="H135" s="8"/>
-      <c r="I135" s="8"/>
-      <c r="J135" s="8"/>
-    </row>
-    <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B136" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C136" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D136" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E136" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F136" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G136" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H136" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I136" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="J136" s="8"/>
-    </row>
-    <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B137" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C137" s="8"/>
-      <c r="D137" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E137" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F137" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="G137" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H137" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I137" s="8"/>
-      <c r="J137" s="8"/>
-    </row>
-    <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B138" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C138" s="8"/>
-      <c r="D138" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E138" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F138" s="7" t="n">
-        <v>1000000000</v>
-      </c>
-      <c r="G138" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H138" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I138" s="8"/>
-      <c r="J138" s="8"/>
-    </row>
-    <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="8"/>
-      <c r="B139" s="8"/>
-      <c r="C139" s="8"/>
-      <c r="D139" s="8"/>
-      <c r="E139" s="8"/>
-      <c r="F139" s="8"/>
-      <c r="G139" s="8"/>
-      <c r="H139" s="8"/>
-      <c r="I139" s="8"/>
-      <c r="J139" s="8"/>
-    </row>
-    <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B140" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="C140" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D140" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E140" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F140" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G140" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H140" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I140" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="J140" s="8"/>
-    </row>
-    <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B141" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="C141" s="8"/>
-      <c r="D141" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E141" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F141" s="7" t="n">
-        <v>1500000000</v>
-      </c>
-      <c r="G141" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H141" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I141" s="8"/>
-      <c r="J141" s="8"/>
-    </row>
-    <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="8"/>
-      <c r="B142" s="8"/>
-      <c r="C142" s="8"/>
-      <c r="D142" s="8"/>
-      <c r="E142" s="8"/>
-      <c r="F142" s="8"/>
-      <c r="G142" s="8"/>
-      <c r="H142" s="8"/>
-      <c r="I142" s="8"/>
-      <c r="J142" s="8"/>
-    </row>
-    <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B143" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="C143" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D143" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E143" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F143" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G143" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H143" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I143" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="J143" s="8"/>
-    </row>
-    <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B144" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="C144" s="8"/>
-      <c r="D144" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E144" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F144" s="7" t="n">
-        <v>3500000000</v>
-      </c>
-      <c r="G144" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H144" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I144" s="8"/>
-      <c r="J144" s="8"/>
-    </row>
-    <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="8"/>
-      <c r="B145" s="8"/>
-      <c r="C145" s="8"/>
-      <c r="D145" s="8"/>
-      <c r="E145" s="8"/>
-      <c r="F145" s="8"/>
-      <c r="G145" s="8"/>
-      <c r="H145" s="8"/>
-      <c r="I145" s="8"/>
-      <c r="J145" s="8"/>
-    </row>
-    <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B146" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C146" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D146" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E146" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F146" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G146" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H146" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I146" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="J146" s="8"/>
-    </row>
-    <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B147" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C147" s="8"/>
-      <c r="D147" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E147" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F147" s="7" t="n">
-        <v>1500000000</v>
-      </c>
-      <c r="G147" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H147" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I147" s="8"/>
-      <c r="J147" s="8"/>
-    </row>
-    <row r="148" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="8"/>
-      <c r="B148" s="8"/>
-      <c r="C148" s="8"/>
-      <c r="D148" s="8"/>
-      <c r="E148" s="8"/>
-      <c r="F148" s="8"/>
-      <c r="G148" s="8"/>
-      <c r="H148" s="8"/>
-      <c r="I148" s="8"/>
-      <c r="J148" s="8"/>
-    </row>
-    <row r="149" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B149" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C149" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D149" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E149" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F149" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G149" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H149" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I149" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J149" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="N149" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B150" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C150" s="8"/>
-      <c r="D150" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E150" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F150" s="7" t="n">
-        <v>1500000000</v>
-      </c>
-      <c r="G150" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H150" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I150" s="8"/>
-      <c r="J150" s="8"/>
-    </row>
-    <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="8"/>
-      <c r="B151" s="8"/>
-      <c r="C151" s="8"/>
-      <c r="D151" s="8"/>
-      <c r="E151" s="8"/>
-      <c r="F151" s="8"/>
-      <c r="G151" s="8"/>
-      <c r="H151" s="8"/>
-      <c r="I151" s="8"/>
-      <c r="J151" s="8"/>
-    </row>
-    <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B152" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C152" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D152" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E152" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F152" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G152" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H152" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I152" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="J152" s="8"/>
-    </row>
-    <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B153" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C153" s="8"/>
-      <c r="D153" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E153" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F153" s="7" t="n">
-        <v>3500000000</v>
-      </c>
-      <c r="G153" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H153" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I153" s="8"/>
-      <c r="J153" s="8"/>
-    </row>
-    <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="8"/>
-      <c r="B154" s="8"/>
-      <c r="C154" s="8"/>
-      <c r="D154" s="8"/>
-      <c r="E154" s="8"/>
-      <c r="F154" s="8"/>
-      <c r="G154" s="8"/>
-      <c r="H154" s="8"/>
-      <c r="I154" s="8"/>
-      <c r="J154" s="8"/>
-    </row>
-    <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B155" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C155" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D155" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E155" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F155" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G155" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H155" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I155" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="J155" s="8"/>
-    </row>
-    <row r="156" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B156" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C156" s="8"/>
-      <c r="D156" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E156" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F156" s="7" t="n">
-        <v>1500000000</v>
-      </c>
-      <c r="G156" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H156" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I156" s="8"/>
-      <c r="J156" s="8"/>
-    </row>
-    <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="8"/>
-      <c r="B157" s="8"/>
-      <c r="C157" s="8"/>
-      <c r="D157" s="8"/>
-      <c r="E157" s="8"/>
-      <c r="F157" s="8"/>
-      <c r="G157" s="8"/>
-      <c r="H157" s="8"/>
-      <c r="I157" s="8"/>
-      <c r="J157" s="8"/>
-    </row>
-    <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B158" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C158" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D158" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E158" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F158" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="G158" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H158" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I158" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="J158" s="8"/>
-    </row>
-    <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B159" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C159" s="8"/>
-      <c r="D159" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E159" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F159" s="7" t="n">
-        <v>10000</v>
-      </c>
-      <c r="G159" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H159" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I159" s="8"/>
-      <c r="J159" s="8"/>
-    </row>
+      <c r="G160" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H160" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I160" s="4"/>
+      <c r="J160" s="4"/>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -4456,7 +4532,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F136 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="S88:S90 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4479,7 +4555,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F136 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="S88:S90 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>